<commit_message>
Action class and write/read excel file uploaded
</commit_message>
<xml_diff>
--- a/Volaris/InspectedWebElements/ListOfInspectedWebElements.xlsx
+++ b/Volaris/InspectedWebElements/ListOfInspectedWebElements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>Domestic flight Card Payment in MXN currency with baggage and trip extras</t>
   </si>
@@ -35,9 +35,6 @@
     <t>opc</t>
   </si>
   <si>
-    <t>InspectID</t>
-  </si>
-  <si>
     <t>input_origin</t>
   </si>
   <si>
@@ -62,15 +59,9 @@
     <t>form-control btn btn-default dropdown-toggle roundTripSelect</t>
   </si>
   <si>
-    <t>css=a:contains("Round trip")</t>
-  </si>
-  <si>
     <t>css_DropDownRoundTrip</t>
   </si>
   <si>
-    <t>css=a:contains("One way")</t>
-  </si>
-  <si>
     <t>css_DropDownOneWay</t>
   </si>
   <si>
@@ -153,6 +144,231 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>submit_search_button</t>
+  </si>
+  <si>
+    <t>id_NextButtonOnReturnFlight</t>
+  </si>
+  <si>
+    <t>js-bundle-modal-option</t>
+  </si>
+  <si>
+    <t>class_NoThanksOnComboPopUp</t>
+  </si>
+  <si>
+    <t>id_FirstNameTextbox</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Name_First</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Name_Middle</t>
+  </si>
+  <si>
+    <t>id_MiddleNameTextbox</t>
+  </si>
+  <si>
+    <t>id_LastNameTextbox</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Name_Last</t>
+  </si>
+  <si>
+    <t>id_MonthDOB</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__month</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__day</t>
+  </si>
+  <si>
+    <t>id_DayDOB</t>
+  </si>
+  <si>
+    <t>id_YearDOB</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__year</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Info_Nationality</t>
+  </si>
+  <si>
+    <t>id_Nationality</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Info_Gender_Male</t>
+  </si>
+  <si>
+    <t>id_GenderMale</t>
+  </si>
+  <si>
+    <t>volarisPassengers_0__Info_Gender_Female</t>
+  </si>
+  <si>
+    <t>id_GenderFemale</t>
+  </si>
+  <si>
+    <t>More flexibility combo</t>
+  </si>
+  <si>
+    <t>linkText_MoreFlexible</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[1]/div/div[1]/div/div[1]/div[2]/a</t>
+  </si>
+  <si>
+    <t>XPath_DetailsMoreFlexible</t>
+  </si>
+  <si>
+    <t>More baggage combo</t>
+  </si>
+  <si>
+    <t>linkText_MoreBaggage</t>
+  </si>
+  <si>
+    <t>XPath_DetailsMoreBaggage</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[2]/div/div[1]/div/div[2]/div[2]/a</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[1]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>XPath_CloaseDetailsMoreFlexible</t>
+  </si>
+  <si>
+    <t>XPath_CloaseDetailsMoreBaggage</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[2]/div/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>More speed combo</t>
+  </si>
+  <si>
+    <t>linkText_MoreSpeed</t>
+  </si>
+  <si>
+    <t>XPath_DetailsMoreSpeed</t>
+  </si>
+  <si>
+    <t>XPath_CloseDetailsMoreSpeed</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[3]/div/div[1]/div/div[1]/div[2]/a</t>
+  </si>
+  <si>
+    <t>//*[@id='carousel-inner-container']/div[3]/div/div[2]/div</t>
+  </si>
+  <si>
+    <t>InspectElementID</t>
+  </si>
+  <si>
+    <t>View Special Assistance &amp; Pet Option</t>
+  </si>
+  <si>
+    <t>linkText_ViewAssistanceAndPetOption</t>
+  </si>
+  <si>
+    <t>class_AddWheelchair</t>
+  </si>
+  <si>
+    <t>checkbox-passenger checkbox</t>
+  </si>
+  <si>
+    <t>id_SelectDog</t>
+  </si>
+  <si>
+    <t>PaxSsrs-PetDog</t>
+  </si>
+  <si>
+    <t>id_SelectCat</t>
+  </si>
+  <si>
+    <t>PaxSsrs-PetCat</t>
+  </si>
+  <si>
+    <t>radio pet-location-radio radio-overlay</t>
+  </si>
+  <si>
+    <t>class_OnBoard</t>
+  </si>
+  <si>
+    <t>class_OnBelly</t>
+  </si>
+  <si>
+    <t>radio pet-location-radio radio-overlay checked radio-selected</t>
+  </si>
+  <si>
+    <t>Hide Special Assistance &amp; Pet Option</t>
+  </si>
+  <si>
+    <t>linkText_HideAssistanceAndPetOption</t>
+  </si>
+  <si>
+    <t>ca:contains("Round trip")</t>
+  </si>
+  <si>
+    <t>a:contains("One way")</t>
+  </si>
+  <si>
+    <t>span:contains("Use FIRST passenger's")</t>
+  </si>
+  <si>
+    <t>css_UseFirstPassenger</t>
+  </si>
+  <si>
+    <t>volarisContact_Name_First</t>
+  </si>
+  <si>
+    <t>id_FirstNameContact</t>
+  </si>
+  <si>
+    <t>id_LastNameContact</t>
+  </si>
+  <si>
+    <t>volarisContact_Name_Last</t>
+  </si>
+  <si>
+    <t>volarisContact_EmailAddress</t>
+  </si>
+  <si>
+    <t>id_Email</t>
+  </si>
+  <si>
+    <t>volarisContact_VerifyEmailAddress</t>
+  </si>
+  <si>
+    <t>id_VerifyEmail</t>
+  </si>
+  <si>
+    <t>dropdownMenu1</t>
+  </si>
+  <si>
+    <t>id_CountryCode</t>
+  </si>
+  <si>
+    <t>volarisContact_HomePhone</t>
+  </si>
+  <si>
+    <t>id_PhoneNumber</t>
+  </si>
+  <si>
+    <t>//*[@id='passengerForm']/div[2]/div/div/div/div/label[1]/span</t>
+  </si>
+  <si>
+    <t>Xpath_AcceptCheckbox</t>
+  </si>
+  <si>
+    <t>submit_passenger_button</t>
+  </si>
+  <si>
+    <t>id_NextSubmitButton</t>
   </si>
 </sst>
 </file>
@@ -480,15 +696,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,10 +721,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,162 +737,450 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>